<commit_message>
refined subdata and guilaunch.Init() to init eel
</commit_message>
<xml_diff>
--- a/data/Subdata.xlsx
+++ b/data/Subdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senio\Documents\Programming\Python Scripts\VSCode\AGE\Class\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968E107F-5644-4768-95E7-EB51E7DB9849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D7E526-B513-466B-8DFF-D230D782AD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{1679E72E-8A18-944B-B572-A65605D2AF7D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -53,57 +53,30 @@
     <t>#99 Grand Slam Ham</t>
   </si>
   <si>
-    <t>33% MORE ham, 2x provolone, lettuce, tomatoes, onions, and mayo</t>
-  </si>
-  <si>
     <t>#15 Titan Turkey</t>
   </si>
   <si>
-    <t>33% MORE* turkey, 2x provolone, lettuce, tomatoes, onions, and mayo</t>
-  </si>
-  <si>
     <t>#17 Garlic Roast Beef</t>
   </si>
   <si>
-    <t>roast beef, 2x provolone, lettuce, tomatoes, onions, and Roasted Garlic Aioli</t>
-  </si>
-  <si>
     <t>#30 The Beast</t>
   </si>
   <si>
-    <t>pepperoni, salami, turkey, ham and roast beef, 2x provolone, lettuce, tomatoes, onions, mayo, and MVP Vinaigrette</t>
-  </si>
-  <si>
     <t>#1 The Philly</t>
   </si>
   <si>
-    <t>steak, 2x American Cheese, Green Peppers, Red Onions, Toasted, and Mayo</t>
-  </si>
-  <si>
     <t>#33 Teriyaki Blitz</t>
   </si>
   <si>
-    <t>steak, 2x American Cheese, Green Peppers, Red Onions, Toasted, and Sweet Onion Teriyaki sauce</t>
-  </si>
-  <si>
     <t>#2 The Outlaw</t>
   </si>
   <si>
-    <t>steak, 2x pepperjack cheese, green peppers, red onions, baja chiptole sauce, Toasted</t>
-  </si>
-  <si>
     <t>#3 The Monster</t>
   </si>
   <si>
-    <t>juicy steak, crisp bacon, a double helping of Monterey cheddar, green peppers and red onions piled high and served toasted on Artisan Italian bread and topped off with creamy Peppercorn Ranch</t>
-  </si>
-  <si>
     <t>#4 Supreme Meats</t>
   </si>
   <si>
-    <t>Black Forest ham, Genoa salami, pepperoni, and our NEW capicola on fresh-baked Artisan Italian bread with provolone cheese, lettuce, tomatoes, red onions, and banana peppers</t>
-  </si>
-  <si>
     <t>Genoa salami, spicy pepperoni, savory Black Forest ham, provolone cheese, crisp lettuce, tomatoes, red onions</t>
   </si>
   <si>
@@ -113,42 +86,21 @@
     <t>#5 Bella Mozza</t>
   </si>
   <si>
-    <t>Thin-sliced Black Forest ham, our NEW capicola, and BelGioioso® Fresh Mozzarella on fresh-baked Artisan Italian bread. Topped with spinach, tomatoes, red onions, and banana peppers</t>
-  </si>
-  <si>
     <t>#6 The Boss</t>
   </si>
   <si>
-    <t>uicy meatballs drenched in marinara sauce with slices of pepperoni and BelGioioso® Fresh Mozzarella</t>
-  </si>
-  <si>
     <t>#8 The Great Garlic</t>
   </si>
   <si>
-    <t xml:space="preserve">juicy rotisserie-style chicken, crispy bacon, provolone, lettuce, tomatoes, red onions </t>
-  </si>
-  <si>
     <t>#16 All-Pro Sweet Onion Teriyaki</t>
   </si>
   <si>
-    <t>toasted Hearty Multigrain bread, tender grilled chicken strips marinated in our Sweet Onion Teriyaki sauce, American cheese, lettuce, tomatoes, and red onions.</t>
-  </si>
-  <si>
     <t>#20 Elite Chicken &amp; Bacon Ranch</t>
   </si>
   <si>
-    <t>tender rotisserie-style chicken, melted Monterey cheddar cheese, hickory-smoked bacon, lettuce, tomatoes, red onions,</t>
-  </si>
-  <si>
     <t>#9 The Champ</t>
   </si>
   <si>
-    <t>Tender hand-pulled rotisserie-style chicken, a double helping of Monterey Cheddar, green peppers, and red onions</t>
-  </si>
-  <si>
-    <t>juicy rotisserie-style chicken, smashed avocado, double Pepper Jack cheese, lettuce, tomatoes, and red onions</t>
-  </si>
-  <si>
     <t>#10 All-American Club</t>
   </si>
   <si>
@@ -161,9 +113,6 @@
     <t>#11 Subway Club</t>
   </si>
   <si>
-    <t>Oven-roasted turkey, Black Forest ham, USDA Choice Roast Beef, provolone cheese piled on Hearty Multigrain bread and topped with lettuce, tomatoes, red onions, and mayo</t>
-  </si>
-  <si>
     <t>#12 Turkey Cali Club</t>
   </si>
   <si>
@@ -174,6 +123,60 @@
   </si>
   <si>
     <t>#7 The Mexicali</t>
+  </si>
+  <si>
+    <t>Juicy meatballs drenched in marinara sauce with slices of pepperoni and BelGioioso® Fresh Mozzarella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juicy rotisserie-style chicken, crispy bacon, provolone, lettuce, tomatoes, red onions </t>
+  </si>
+  <si>
+    <t>Tender rotisserie-style chicken, melted Monterey cheddar cheese, hickory-smoked bacon, lettuce, tomatoes, red onions,</t>
+  </si>
+  <si>
+    <t>Juicy rotisserie-style chicken, smashed avocado, double Pepper Jack cheese, lettuce, tomatoes, and red onions</t>
+  </si>
+  <si>
+    <t>Roast beef, 2x provolone, lettuce, tomatoes, onions, and Roasted Garlic Aioli</t>
+  </si>
+  <si>
+    <t>Pepperoni, salami, turkey, ham and roast beef, 2x provolone, lettuce, tomatoes, onions, mayo, and MVP Vinaigrette</t>
+  </si>
+  <si>
+    <t>Steak, 2x American Cheese, Green Peppers, Red Onions, Toasted, and Mayo</t>
+  </si>
+  <si>
+    <t>Steak, 2x American Cheese, Green Peppers, Red Onions, Toasted, and Sweet Onion Teriyaki sauce</t>
+  </si>
+  <si>
+    <t>Steak, 2x pepperjack cheese, green peppers, red onions, baja chiptole sauce, Toasted</t>
+  </si>
+  <si>
+    <t>Steak, bacon, Monterey cheddar, green peppers and red onions piled high, Artisan Italian bread, creamy Peppercorn Ranch</t>
+  </si>
+  <si>
+    <t>Black Forest ham, Genoa salami, pepperoni, capicola on Italian bread with provolone cheese, lettuce, tomatoes, red onions, and banana peppers</t>
+  </si>
+  <si>
+    <t>Genoa salami, spicy pepperoni, jalapeno peppers, lettuce, tomato, red onions, provolone cheese, and MVP Parmesan Vinaigrette</t>
+  </si>
+  <si>
+    <t>Thin-sliced Black Forest ham, capicola, and BelGioioso® Fresh Mozzarella on Italian bread; with spinach, tomatoes, red onions, and banana peppers</t>
+  </si>
+  <si>
+    <t>Multigrain bread, grilled chicken strips marinated in Sweet Onion Teriyaki sauce, American cheese, lettuce, tomatoes, and red onions.</t>
+  </si>
+  <si>
+    <t>Tender hand-pulled rotisserie-style chicken, Monterey Cheddar, green peppers, and red onions</t>
+  </si>
+  <si>
+    <t>Oven-roasted turkey, Black Forest ham, Roast Beef, provolone cheese on Multigrain bread topped with lettuce, tomatoes, red onions, and mayo</t>
+  </si>
+  <si>
+    <t>Ham, provolone, lettuce, tomatoes, onions, and mayo</t>
+  </si>
+  <si>
+    <t>Turkey, provolone, lettuce, tomatoes, onions, and mayo</t>
   </si>
 </sst>
 </file>
@@ -568,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1C98EE-A01B-7547-A092-4344E54CDA46}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -590,23 +593,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="46.5">
+    <row r="2" spans="1:3" ht="31">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2">
         <v>6.39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.5">
+    <row r="3" spans="1:3" ht="31">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
         <v>6.79</v>
@@ -614,10 +617,10 @@
     </row>
     <row r="4" spans="1:3" ht="46.5">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
         <v>6.79</v>
@@ -625,10 +628,10 @@
     </row>
     <row r="5" spans="1:3" ht="62">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2">
         <v>7.89</v>
@@ -636,10 +639,10 @@
     </row>
     <row r="6" spans="1:3" ht="46.5">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2">
         <v>6.69</v>
@@ -647,10 +650,10 @@
     </row>
     <row r="7" spans="1:3" ht="46.5">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2">
         <v>6.69</v>
@@ -658,32 +661,32 @@
     </row>
     <row r="8" spans="1:3" ht="46.5">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2">
         <v>6.69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="108.5">
+    <row r="9" spans="1:3" ht="62">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2">
         <v>7.19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="93">
+    <row r="10" spans="1:3" ht="77.5">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2">
         <v>6.19</v>
@@ -691,32 +694,32 @@
     </row>
     <row r="11" spans="1:3" ht="62">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <v>5.59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="93">
+    <row r="12" spans="1:3" ht="77.5">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2">
         <v>6.19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="93">
+    <row r="13" spans="1:3" ht="77.5">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2">
         <v>6.19</v>
@@ -724,10 +727,10 @@
     </row>
     <row r="14" spans="1:3" ht="62">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
         <v>5.99</v>
@@ -735,21 +738,21 @@
     </row>
     <row r="15" spans="1:3" ht="46.5">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
         <v>6.59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="93">
+    <row r="16" spans="1:3" ht="77.5">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2">
         <v>5.99</v>
@@ -757,21 +760,21 @@
     </row>
     <row r="17" spans="1:3" ht="31">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2">
         <v>6.59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="62">
+    <row r="18" spans="1:3" ht="46.5">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>6.29</v>
@@ -779,10 +782,10 @@
     </row>
     <row r="19" spans="1:3" ht="62">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2">
         <v>6.69</v>
@@ -790,10 +793,10 @@
     </row>
     <row r="20" spans="1:3" ht="62">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
         <v>6.39</v>
@@ -801,21 +804,21 @@
     </row>
     <row r="21" spans="1:3" ht="62">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2">
         <v>5.99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="93">
+    <row r="22" spans="1:3" ht="77.5">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C22" s="2">
         <v>6.59</v>
@@ -823,10 +826,10 @@
     </row>
     <row r="23" spans="1:3" ht="77.5">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2">
         <v>10.39</v>

</xml_diff>